<commit_message>
Add favicons, polish text before first publish
</commit_message>
<xml_diff>
--- a/ideas/just-start/just-start.xlsx
+++ b/ideas/just-start/just-start.xlsx
@@ -72,7 +72,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,10 +116,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1361,8 +1368,8 @@
       <xdr:rowOff>9526</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>9526</xdr:rowOff>
     </xdr:to>
@@ -1380,7 +1387,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="6105526"/>
-          <a:ext cx="17964150" cy="4572000"/>
+          <a:ext cx="14239875" cy="4572000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1749,9 +1756,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>640445</xdr:colOff>
+      <xdr:colOff>297545</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>146420</xdr:rowOff>
+      <xdr:rowOff>174995</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5007076" cy="790922"/>
     <xdr:sp macro="" textlink="">
@@ -1767,7 +1774,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4850495" y="4146920"/>
+          <a:off x="4507595" y="4175495"/>
           <a:ext cx="5007076" cy="790922"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2337,8 +2344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2493,7 +2500,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" ref="E4:E8" si="4">E5+5</f>
+        <f t="shared" ref="E6:E8" si="4">E5+5</f>
         <v>5</v>
       </c>
       <c r="F6" s="1">

</xml_diff>

<commit_message>
More just start refinement, start of ask why idea
</commit_message>
<xml_diff>
--- a/ideas/just-start/just-start.xlsx
+++ b/ideas/just-start/just-start.xlsx
@@ -1474,11 +1474,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>694897</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>76595</xdr:rowOff>
+      <xdr:colOff>606968</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>24173</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1538498" cy="511422"/>
+    <xdr:ext cx="1200008" cy="406714"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="6" name="TextBox 5">
@@ -1492,8 +1492,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="21412180">
-          <a:off x="10391347" y="2362595"/>
-          <a:ext cx="1538498" cy="511422"/>
+          <a:off x="10303418" y="2500673"/>
+          <a:ext cx="1200008" cy="406714"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1521,7 +1521,7 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-ZA" sz="2400" b="1">
+            <a:rPr lang="en-ZA" sz="1800" b="1">
               <a:solidFill>
                 <a:srgbClr val="00B050"/>
               </a:solidFill>
@@ -1539,11 +1539,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1408459</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>144082</xdr:rowOff>
+      <xdr:colOff>1317939</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>141876</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="511422" cy="1538498"/>
+    <xdr:ext cx="406714" cy="1200008"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="7" name="TextBox 6">
@@ -1557,8 +1557,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="18736574">
-          <a:off x="10591371" y="3324620"/>
-          <a:ext cx="1538498" cy="511422"/>
+          <a:off x="10617742" y="3586523"/>
+          <a:ext cx="1200008" cy="406714"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1586,7 +1586,7 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-ZA" sz="2400" b="1">
+            <a:rPr lang="en-ZA" sz="1800" b="1">
               <a:solidFill>
                 <a:srgbClr val="0070C0"/>
               </a:solidFill>
@@ -1604,11 +1604,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>690927</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>38430</xdr:rowOff>
+      <xdr:colOff>1607729</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>359</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="3854838" cy="651204"/>
+    <xdr:ext cx="2478435" cy="441596"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="8" name="TextBox 7">
@@ -1622,8 +1622,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="21020158">
-          <a:off x="8558577" y="5372430"/>
-          <a:ext cx="3854838" cy="651204"/>
+          <a:off x="9475379" y="5715359"/>
+          <a:ext cx="2478435" cy="441596"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1651,7 +1651,7 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-ZA" sz="3200" b="1">
+            <a:rPr lang="en-ZA" sz="2000" b="1">
               <a:solidFill>
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
@@ -1662,7 +1662,7 @@
             <a:t>Working</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-ZA" sz="3200" b="1" baseline="0">
+            <a:rPr lang="en-ZA" sz="2000" b="1" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
@@ -1673,7 +1673,7 @@
             <a:t> </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-ZA" sz="3200" b="1">
+            <a:rPr lang="en-ZA" sz="2000" b="1">
               <a:solidFill>
                 <a:schemeClr val="bg1"/>
               </a:solidFill>
@@ -1690,18 +1690,18 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1187712</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>22597</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>116570</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>32120</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1453860" cy="651204"/>
+    <xdr:ext cx="6058966" cy="930639"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="TextBox 8">
+        <xdr:cNvPr id="12" name="TextBox 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BD1D34E-0D43-4391-9E56-4C6ED3393A7A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8138FF5A-1621-4E5A-AFAA-30EA6725FE0C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1709,8 +1709,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10884162" y="7071097"/>
-          <a:ext cx="1453860" cy="651204"/>
+          <a:off x="4326620" y="4032620"/>
+          <a:ext cx="6058966" cy="930639"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1738,72 +1738,7 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-ZA" sz="3200" b="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-              <a:latin typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Waste</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>297545</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>174995</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="5007076" cy="790922"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="TextBox 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8138FF5A-1621-4E5A-AFAA-30EA6725FE0C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4507595" y="4175495"/>
-          <a:ext cx="5007076" cy="790922"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-ZA" sz="4000" b="1">
+            <a:rPr lang="en-ZA" sz="4800" b="1">
               <a:solidFill>
                 <a:srgbClr val="00B050"/>
               </a:solidFill>
@@ -1822,7 +1757,7 @@
               <a:ea typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
               <a:cs typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t> </a:t>
+            <a:t>  </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-ZA" sz="3200" b="1" i="1" baseline="0">
@@ -1835,10 +1770,10 @@
               <a:ea typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
               <a:cs typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>vs. </a:t>
+            <a:t>vs.  </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-ZA" sz="4000" b="1" baseline="0">
+            <a:rPr lang="en-ZA" sz="4800" b="1" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="0070C0"/>
               </a:solidFill>
@@ -1923,6 +1858,142 @@
               <a:cs typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>Time</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1006737</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>13072</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="832664" cy="406714"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="TextBox 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E89468D-FAB8-4C4B-B7E2-3C852C00C514}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1559187" y="2489572"/>
+          <a:ext cx="832664" cy="406714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-ZA" sz="1800" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Value</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>978162</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>136897</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="898516" cy="406714"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5081F360-AA05-47F5-A983-A98B4555FAAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1530612" y="8328397"/>
+          <a:ext cx="898516" cy="406714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-ZA" sz="1800" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Open Sans" panose="020B0606030504020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Waste</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2344,8 +2415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>